<commit_message>
Jatai changed files 12/08/2019
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6372"/>
+    <workbookView visibility="hidden" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6372"/>
   </bookViews>
   <sheets>
     <sheet name="TS 4.5" sheetId="1" r:id="rId1"/>
@@ -3803,7 +3803,7 @@
       <selection activeCell="K1" sqref="K1"/>
       <selection pane="topRight" activeCell="P1" sqref="P1"/>
       <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
-      <selection pane="bottomRight" activeCell="AE20" sqref="AE20"/>
+      <selection pane="bottomRight" sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
TS Kramam 2.4 & 2.5 Tamil corr 13/11/2019
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="hidden" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6372"/>
   </bookViews>
   <sheets>
     <sheet name="TS 4.5" sheetId="1" r:id="rId1"/>
@@ -3798,12 +3798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK634"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="K1" sqref="K1"/>
-      <selection pane="topRight" activeCell="P1" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
-      <selection pane="bottomRight" sqref="A1:L1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Corrections for Raja 31/05/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Padam Input Template.xlsx
+++ b/TS Jatai Working/Padam Input Template.xlsx
@@ -5474,9 +5474,6 @@
     <t xml:space="preserve">Uqrddhva u# vUqrddhva Uqrddhva u# | </t>
   </si>
   <si>
-    <t xml:space="preserve"> Uqrddhva u# vUqrddhva Uqrddhva Uq Shu No# naqs sU vUqrddhva Uq Shu Na#H |</t>
-  </si>
-  <si>
     <t>Shu No# naqs sU Shu Na#H |</t>
   </si>
   <si>
@@ -5859,6 +5856,9 @@
   </si>
   <si>
     <t xml:space="preserve">dIqrGAqyuqtvAyeti# dIrGAyu - tvAya# </t>
+  </si>
+  <si>
+    <t>Uqrddhva u# vUqrddhva Uqrddhva Uq Shu No# naqs sU vUqrddhva Uq Shu Na#H |</t>
   </si>
 </sst>
 </file>
@@ -6453,11 +6453,11 @@
   <dimension ref="A1:AK668"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AI3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
       <selection pane="topRight" activeCell="N1" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomRight" activeCell="AI334" sqref="AI334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -12355,7 +12355,7 @@
       <c r="P88" s="33"/>
       <c r="Q88" s="33"/>
       <c r="R88" s="33" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="S88" s="33"/>
       <c r="T88" s="33"/>
@@ -13225,10 +13225,10 @@
       <c r="S103" s="15"/>
       <c r="T103" s="15"/>
       <c r="U103" s="62" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="V103" s="15" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="W103" s="15"/>
       <c r="X103" s="15"/>
@@ -13757,7 +13757,7 @@
       <c r="K113" s="13"/>
       <c r="L113" s="13"/>
       <c r="M113" s="8" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="N113" s="14"/>
       <c r="O113" s="14"/>
@@ -13788,7 +13788,7 @@
       <c r="K114" s="13"/>
       <c r="L114" s="13"/>
       <c r="M114" s="8" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="N114" s="14"/>
       <c r="O114" s="14"/>
@@ -13819,7 +13819,7 @@
       <c r="K115" s="13"/>
       <c r="L115" s="13"/>
       <c r="M115" s="8" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="N115" s="14"/>
       <c r="O115" s="14"/>
@@ -13850,7 +13850,7 @@
       <c r="K116" s="13"/>
       <c r="L116" s="13"/>
       <c r="M116" s="8" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="N116" s="14"/>
       <c r="O116" s="14"/>
@@ -13883,7 +13883,7 @@
       <c r="K117" s="13"/>
       <c r="L117" s="13"/>
       <c r="M117" s="8" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="N117" s="14"/>
       <c r="O117" s="14"/>
@@ -13914,7 +13914,7 @@
       <c r="K118" s="13"/>
       <c r="L118" s="13"/>
       <c r="M118" s="8" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="N118" s="14"/>
       <c r="O118" s="14" t="s">
@@ -13938,7 +13938,7 @@
       <c r="AE118" s="15"/>
       <c r="AF118" s="15"/>
       <c r="AG118" s="33" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="AH118" s="43"/>
       <c r="AI118" s="43"/>
@@ -14146,7 +14146,7 @@
       </c>
       <c r="S122" s="15"/>
       <c r="T122" s="15" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="U122" s="15"/>
       <c r="V122" s="15"/>
@@ -14581,7 +14581,7 @@
       <c r="K131" s="13"/>
       <c r="L131" s="13"/>
       <c r="M131" s="8" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="N131" s="14"/>
       <c r="O131" s="15"/>
@@ -14604,10 +14604,10 @@
       <c r="AF131" s="15"/>
       <c r="AG131" s="16"/>
       <c r="AH131" s="43" t="s">
+        <v>1872</v>
+      </c>
+      <c r="AI131" s="43" t="s">
         <v>1873</v>
-      </c>
-      <c r="AI131" s="43" t="s">
-        <v>1874</v>
       </c>
     </row>
     <row r="132" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -14616,7 +14616,7 @@
       <c r="K132" s="13"/>
       <c r="L132" s="13"/>
       <c r="M132" s="8" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="N132" s="14"/>
       <c r="O132" s="15"/>
@@ -14639,10 +14639,10 @@
       <c r="AF132" s="15"/>
       <c r="AG132" s="16"/>
       <c r="AH132" s="43" t="s">
+        <v>1874</v>
+      </c>
+      <c r="AI132" s="43" t="s">
         <v>1875</v>
-      </c>
-      <c r="AI132" s="43" t="s">
-        <v>1876</v>
       </c>
     </row>
     <row r="133" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -14651,7 +14651,7 @@
       <c r="K133" s="13"/>
       <c r="L133" s="13"/>
       <c r="M133" s="8" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="N133" s="14"/>
       <c r="O133" s="15"/>
@@ -14674,10 +14674,10 @@
       <c r="AF133" s="15"/>
       <c r="AG133" s="16"/>
       <c r="AH133" s="43" t="s">
+        <v>1876</v>
+      </c>
+      <c r="AI133" s="43" t="s">
         <v>1877</v>
-      </c>
-      <c r="AI133" s="43" t="s">
-        <v>1878</v>
       </c>
     </row>
     <row r="134" spans="1:35" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -14686,7 +14686,7 @@
       <c r="K134" s="13"/>
       <c r="L134" s="13"/>
       <c r="M134" s="8" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="N134" s="14"/>
       <c r="O134" s="15"/>
@@ -14709,7 +14709,7 @@
       <c r="AF134" s="15"/>
       <c r="AG134" s="16"/>
       <c r="AH134" s="43" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="AI134" s="43"/>
     </row>
@@ -14719,7 +14719,7 @@
       <c r="K135" s="13"/>
       <c r="L135" s="13"/>
       <c r="M135" s="8" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="N135" s="14"/>
       <c r="O135" s="15" t="s">
@@ -14743,7 +14743,7 @@
       <c r="AE135" s="15"/>
       <c r="AF135" s="15"/>
       <c r="AG135" s="16" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="AH135" s="43"/>
       <c r="AI135" s="43"/>
@@ -14754,7 +14754,7 @@
       <c r="K136" s="13"/>
       <c r="L136" s="13"/>
       <c r="M136" s="8" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="N136" s="14"/>
       <c r="O136" s="15"/>
@@ -14777,10 +14777,10 @@
       <c r="AF136" s="15"/>
       <c r="AG136" s="16"/>
       <c r="AH136" s="43" t="s">
+        <v>1879</v>
+      </c>
+      <c r="AI136" s="43" t="s">
         <v>1880</v>
-      </c>
-      <c r="AI136" s="43" t="s">
-        <v>1881</v>
       </c>
     </row>
     <row r="137" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -14789,7 +14789,7 @@
       <c r="K137" s="13"/>
       <c r="L137" s="13"/>
       <c r="M137" s="8" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="N137" s="14"/>
       <c r="O137" s="15"/>
@@ -14812,10 +14812,10 @@
       <c r="AF137" s="15"/>
       <c r="AG137" s="16"/>
       <c r="AH137" s="43" t="s">
+        <v>1881</v>
+      </c>
+      <c r="AI137" s="43" t="s">
         <v>1882</v>
-      </c>
-      <c r="AI137" s="43" t="s">
-        <v>1883</v>
       </c>
     </row>
     <row r="138" spans="1:35" s="12" customFormat="1" ht="52.2" x14ac:dyDescent="0.3">
@@ -14824,7 +14824,7 @@
       <c r="K138" s="13"/>
       <c r="L138" s="13"/>
       <c r="M138" s="8" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="N138" s="14"/>
       <c r="O138" s="15"/>
@@ -14847,10 +14847,10 @@
       <c r="AF138" s="15"/>
       <c r="AG138" s="16"/>
       <c r="AH138" s="43" t="s">
+        <v>1883</v>
+      </c>
+      <c r="AI138" s="43" t="s">
         <v>1884</v>
-      </c>
-      <c r="AI138" s="43" t="s">
-        <v>1885</v>
       </c>
     </row>
     <row r="139" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -14859,7 +14859,7 @@
       <c r="K139" s="13"/>
       <c r="L139" s="13"/>
       <c r="M139" s="8" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="N139" s="14"/>
       <c r="O139" s="15"/>
@@ -14882,7 +14882,7 @@
       <c r="AF139" s="15"/>
       <c r="AG139" s="16"/>
       <c r="AH139" s="43" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="AI139" s="43"/>
     </row>
@@ -14916,7 +14916,7 @@
       <c r="AE140" s="15"/>
       <c r="AF140" s="15"/>
       <c r="AG140" s="16" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="AH140" s="43"/>
       <c r="AI140" s="43"/>
@@ -14927,7 +14927,7 @@
       <c r="K141" s="13"/>
       <c r="L141" s="13"/>
       <c r="M141" s="8" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="N141" s="14"/>
       <c r="O141" s="15"/>
@@ -14950,10 +14950,10 @@
       <c r="AF141" s="15"/>
       <c r="AG141" s="16"/>
       <c r="AH141" s="43" t="s">
+        <v>1886</v>
+      </c>
+      <c r="AI141" s="43" t="s">
         <v>1887</v>
-      </c>
-      <c r="AI141" s="43" t="s">
-        <v>1888</v>
       </c>
     </row>
     <row r="142" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -14962,7 +14962,7 @@
       <c r="K142" s="13"/>
       <c r="L142" s="13"/>
       <c r="M142" s="8" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="N142" s="14"/>
       <c r="O142" s="15"/>
@@ -14985,10 +14985,10 @@
       <c r="AF142" s="15"/>
       <c r="AG142" s="16"/>
       <c r="AH142" s="43" t="s">
+        <v>1888</v>
+      </c>
+      <c r="AI142" s="43" t="s">
         <v>1889</v>
-      </c>
-      <c r="AI142" s="43" t="s">
-        <v>1890</v>
       </c>
     </row>
     <row r="143" spans="1:35" s="12" customFormat="1" ht="52.2" x14ac:dyDescent="0.3">
@@ -14997,7 +14997,7 @@
       <c r="K143" s="13"/>
       <c r="L143" s="13"/>
       <c r="M143" s="8" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="N143" s="14"/>
       <c r="O143" s="15"/>
@@ -15020,10 +15020,10 @@
       <c r="AF143" s="15"/>
       <c r="AG143" s="16"/>
       <c r="AH143" s="43" t="s">
+        <v>1890</v>
+      </c>
+      <c r="AI143" s="43" t="s">
         <v>1891</v>
-      </c>
-      <c r="AI143" s="43" t="s">
-        <v>1892</v>
       </c>
     </row>
     <row r="144" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -15032,7 +15032,7 @@
       <c r="K144" s="13"/>
       <c r="L144" s="13"/>
       <c r="M144" s="8" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="N144" s="14"/>
       <c r="O144" s="15"/>
@@ -15055,10 +15055,10 @@
       <c r="AF144" s="15"/>
       <c r="AG144" s="16"/>
       <c r="AH144" s="43" t="s">
+        <v>1892</v>
+      </c>
+      <c r="AI144" s="43" t="s">
         <v>1893</v>
-      </c>
-      <c r="AI144" s="43" t="s">
-        <v>1894</v>
       </c>
     </row>
     <row r="145" spans="1:35" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -15067,7 +15067,7 @@
       <c r="K145" s="13"/>
       <c r="L145" s="13"/>
       <c r="M145" s="8" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="N145" s="14"/>
       <c r="O145" s="15"/>
@@ -15090,7 +15090,7 @@
       <c r="AF145" s="15"/>
       <c r="AG145" s="16"/>
       <c r="AH145" s="43" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="AI145" s="43"/>
     </row>
@@ -15100,7 +15100,7 @@
       <c r="K146" s="13"/>
       <c r="L146" s="13"/>
       <c r="M146" s="8" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="N146" s="14"/>
       <c r="O146" s="15" t="s">
@@ -15124,7 +15124,7 @@
       <c r="AE146" s="15"/>
       <c r="AF146" s="15"/>
       <c r="AG146" s="16" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="AH146" s="43"/>
       <c r="AI146" s="43"/>
@@ -15135,7 +15135,7 @@
       <c r="K147" s="13"/>
       <c r="L147" s="13"/>
       <c r="M147" s="8" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="N147" s="14"/>
       <c r="O147" s="15"/>
@@ -15158,10 +15158,10 @@
       <c r="AF147" s="15"/>
       <c r="AG147" s="16"/>
       <c r="AH147" s="43" t="s">
+        <v>1900</v>
+      </c>
+      <c r="AI147" s="43" t="s">
         <v>1901</v>
-      </c>
-      <c r="AI147" s="43" t="s">
-        <v>1902</v>
       </c>
     </row>
     <row r="148" spans="1:35" s="12" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.3">
@@ -15170,7 +15170,7 @@
       <c r="K148" s="13"/>
       <c r="L148" s="13"/>
       <c r="M148" s="8" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="N148" s="14"/>
       <c r="O148" s="15"/>
@@ -15193,10 +15193,10 @@
       <c r="AF148" s="15"/>
       <c r="AG148" s="16"/>
       <c r="AH148" s="43" t="s">
+        <v>1902</v>
+      </c>
+      <c r="AI148" s="43" t="s">
         <v>1903</v>
-      </c>
-      <c r="AI148" s="43" t="s">
-        <v>1904</v>
       </c>
     </row>
     <row r="149" spans="1:35" s="12" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.3">
@@ -15205,7 +15205,7 @@
       <c r="K149" s="13"/>
       <c r="L149" s="13"/>
       <c r="M149" s="8" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="N149" s="14"/>
       <c r="O149" s="15"/>
@@ -15228,10 +15228,10 @@
       <c r="AF149" s="15"/>
       <c r="AG149" s="16"/>
       <c r="AH149" s="43" t="s">
+        <v>1904</v>
+      </c>
+      <c r="AI149" s="43" t="s">
         <v>1905</v>
-      </c>
-      <c r="AI149" s="43" t="s">
-        <v>1906</v>
       </c>
     </row>
     <row r="150" spans="1:35" s="12" customFormat="1" ht="52.2" x14ac:dyDescent="0.3">
@@ -15240,7 +15240,7 @@
       <c r="K150" s="13"/>
       <c r="L150" s="13"/>
       <c r="M150" s="8" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="N150" s="14" t="s">
         <v>7</v>
@@ -15264,13 +15264,13 @@
       <c r="AE150" s="15"/>
       <c r="AF150" s="15"/>
       <c r="AG150" s="8" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="AH150" s="43" t="s">
+        <v>1906</v>
+      </c>
+      <c r="AI150" s="43" t="s">
         <v>1907</v>
-      </c>
-      <c r="AI150" s="43" t="s">
-        <v>1908</v>
       </c>
     </row>
     <row r="151" spans="1:35" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -15279,7 +15279,7 @@
       <c r="K151" s="13"/>
       <c r="L151" s="13"/>
       <c r="M151" s="8" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="N151" s="14"/>
       <c r="O151" s="15"/>
@@ -15301,7 +15301,7 @@
       <c r="AE151" s="15"/>
       <c r="AF151" s="15"/>
       <c r="AH151" s="43" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="AI151" s="43"/>
     </row>
@@ -15770,7 +15770,7 @@
       <c r="AE160" s="15"/>
       <c r="AF160" s="15"/>
       <c r="AG160" s="16" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="AH160" s="43" t="s">
         <v>1093</v>
@@ -16333,7 +16333,7 @@
       <c r="AE170" s="15"/>
       <c r="AF170" s="15"/>
       <c r="AG170" s="16" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="AH170" s="43"/>
       <c r="AI170" s="43"/>
@@ -16388,7 +16388,7 @@
         <v>1800</v>
       </c>
       <c r="AI171" s="12" t="s">
-        <v>1801</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="172" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -16511,10 +16511,10 @@
       <c r="AF173" s="15"/>
       <c r="AG173" s="16"/>
       <c r="AH173" s="43" t="s">
+        <v>1801</v>
+      </c>
+      <c r="AI173" s="43" t="s">
         <v>1802</v>
-      </c>
-      <c r="AI173" s="43" t="s">
-        <v>1803</v>
       </c>
     </row>
     <row r="174" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -16561,7 +16561,7 @@
       <c r="X174" s="15"/>
       <c r="Y174" s="15"/>
       <c r="Z174" s="15" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="AA174" s="15"/>
       <c r="AB174" s="15"/>
@@ -17819,7 +17819,7 @@
       <c r="K198" s="13"/>
       <c r="L198" s="13"/>
       <c r="M198" s="8" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="N198" s="14"/>
       <c r="O198" s="15"/>
@@ -17842,10 +17842,10 @@
       <c r="AF198" s="15"/>
       <c r="AG198" s="28"/>
       <c r="AH198" s="43" t="s">
+        <v>1917</v>
+      </c>
+      <c r="AI198" s="43" t="s">
         <v>1918</v>
-      </c>
-      <c r="AI198" s="43" t="s">
-        <v>1919</v>
       </c>
     </row>
     <row r="199" spans="1:35" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -17876,10 +17876,10 @@
       <c r="AF199" s="15"/>
       <c r="AG199" s="28"/>
       <c r="AH199" s="43" t="s">
+        <v>1919</v>
+      </c>
+      <c r="AI199" s="43" t="s">
         <v>1920</v>
-      </c>
-      <c r="AI199" s="43" t="s">
-        <v>1921</v>
       </c>
     </row>
     <row r="200" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -17887,7 +17887,7 @@
       <c r="K200" s="13"/>
       <c r="L200" s="13"/>
       <c r="M200" s="8" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="N200" s="14"/>
       <c r="O200" s="15"/>
@@ -17910,10 +17910,10 @@
       <c r="AF200" s="15"/>
       <c r="AG200" s="28"/>
       <c r="AH200" s="43" t="s">
+        <v>1921</v>
+      </c>
+      <c r="AI200" s="43" t="s">
         <v>1922</v>
-      </c>
-      <c r="AI200" s="43" t="s">
-        <v>1923</v>
       </c>
     </row>
     <row r="201" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -17921,7 +17921,7 @@
       <c r="K201" s="13"/>
       <c r="L201" s="13"/>
       <c r="M201" s="8" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="N201" s="14"/>
       <c r="O201" s="15"/>
@@ -17944,10 +17944,10 @@
       <c r="AF201" s="15"/>
       <c r="AG201" s="28"/>
       <c r="AH201" s="43" t="s">
+        <v>1923</v>
+      </c>
+      <c r="AI201" s="43" t="s">
         <v>1924</v>
-      </c>
-      <c r="AI201" s="43" t="s">
-        <v>1925</v>
       </c>
     </row>
     <row r="202" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -17978,10 +17978,10 @@
       <c r="AF202" s="15"/>
       <c r="AG202" s="28"/>
       <c r="AH202" s="43" t="s">
+        <v>1925</v>
+      </c>
+      <c r="AI202" s="43" t="s">
         <v>1926</v>
-      </c>
-      <c r="AI202" s="43" t="s">
-        <v>1927</v>
       </c>
     </row>
     <row r="203" spans="1:35" s="12" customFormat="1" ht="52.2" x14ac:dyDescent="0.3">
@@ -17989,7 +17989,7 @@
       <c r="K203" s="13"/>
       <c r="L203" s="13"/>
       <c r="M203" s="8" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="N203" s="14"/>
       <c r="O203" s="15"/>
@@ -18012,7 +18012,7 @@
       <c r="AF203" s="15"/>
       <c r="AG203" s="28"/>
       <c r="AH203" s="43" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="AI203" s="43"/>
     </row>
@@ -18021,7 +18021,7 @@
       <c r="K204" s="13"/>
       <c r="L204" s="13"/>
       <c r="M204" s="8" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="N204" s="14" t="s">
         <v>7</v>
@@ -18047,7 +18047,7 @@
       <c r="AE204" s="15"/>
       <c r="AF204" s="15"/>
       <c r="AG204" s="28" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="AH204" s="43"/>
       <c r="AI204" s="43"/>
@@ -18200,10 +18200,10 @@
       <c r="AF207" s="15"/>
       <c r="AG207" s="16"/>
       <c r="AH207" s="43" t="s">
+        <v>1803</v>
+      </c>
+      <c r="AI207" s="43" t="s">
         <v>1804</v>
-      </c>
-      <c r="AI207" s="43" t="s">
-        <v>1805</v>
       </c>
     </row>
     <row r="208" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -18523,10 +18523,10 @@
       <c r="AF213" s="15"/>
       <c r="AG213" s="16"/>
       <c r="AH213" s="43" t="s">
+        <v>1810</v>
+      </c>
+      <c r="AI213" s="43" t="s">
         <v>1811</v>
-      </c>
-      <c r="AI213" s="43" t="s">
-        <v>1812</v>
       </c>
     </row>
     <row r="214" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -18575,10 +18575,10 @@
       <c r="AF214" s="15"/>
       <c r="AG214" s="16"/>
       <c r="AH214" s="43" t="s">
+        <v>1812</v>
+      </c>
+      <c r="AI214" s="43" t="s">
         <v>1813</v>
-      </c>
-      <c r="AI214" s="43" t="s">
-        <v>1814</v>
       </c>
     </row>
     <row r="215" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -19906,10 +19906,10 @@
       <c r="AF239" s="15"/>
       <c r="AG239" s="16"/>
       <c r="AH239" s="43" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="AI239" s="43" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="240" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -19958,10 +19958,10 @@
       <c r="AF240" s="15"/>
       <c r="AG240" s="16"/>
       <c r="AH240" s="43" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="AI240" s="43" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="241" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -20425,7 +20425,7 @@
         <v>1211</v>
       </c>
       <c r="AI249" s="43" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="250" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -21152,10 +21152,10 @@
       <c r="AF263" s="15"/>
       <c r="AG263" s="16"/>
       <c r="AH263" s="43" t="s">
+        <v>1814</v>
+      </c>
+      <c r="AI263" s="43" t="s">
         <v>1815</v>
-      </c>
-      <c r="AI263" s="43" t="s">
-        <v>1816</v>
       </c>
     </row>
     <row r="264" spans="1:35" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -21207,7 +21207,7 @@
         <v>1232</v>
       </c>
       <c r="AI264" s="43" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="265" spans="1:35" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -21800,7 +21800,7 @@
         <v>1247</v>
       </c>
       <c r="AI275" s="43" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="276" spans="1:35" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -21901,10 +21901,10 @@
       <c r="AF277" s="15"/>
       <c r="AG277" s="16"/>
       <c r="AH277" s="43" t="s">
+        <v>1818</v>
+      </c>
+      <c r="AI277" s="43" t="s">
         <v>1819</v>
-      </c>
-      <c r="AI277" s="43" t="s">
-        <v>1820</v>
       </c>
     </row>
     <row r="278" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -22815,7 +22815,7 @@
         <v>1274</v>
       </c>
       <c r="AI294" s="43" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="295" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -23334,10 +23334,10 @@
       <c r="AF304" s="15"/>
       <c r="AG304" s="16"/>
       <c r="AH304" s="43" t="s">
+        <v>1821</v>
+      </c>
+      <c r="AI304" s="43" t="s">
         <v>1822</v>
-      </c>
-      <c r="AI304" s="43" t="s">
-        <v>1823</v>
       </c>
     </row>
     <row r="305" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -23389,7 +23389,7 @@
         <v>1287</v>
       </c>
       <c r="AI305" s="43" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="306" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -23438,7 +23438,7 @@
       <c r="AF306" s="15"/>
       <c r="AG306" s="16"/>
       <c r="AH306" s="43" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="AI306" s="43" t="s">
         <v>1288</v>
@@ -23496,10 +23496,10 @@
       <c r="AF307" s="15"/>
       <c r="AG307" s="16"/>
       <c r="AH307" s="43" t="s">
+        <v>1825</v>
+      </c>
+      <c r="AI307" s="43" t="s">
         <v>1826</v>
-      </c>
-      <c r="AI307" s="43" t="s">
-        <v>1827</v>
       </c>
     </row>
     <row r="308" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -24489,10 +24489,10 @@
       <c r="AF326" s="15"/>
       <c r="AG326" s="16"/>
       <c r="AH326" s="43" t="s">
+        <v>1833</v>
+      </c>
+      <c r="AI326" s="43" t="s">
         <v>1834</v>
-      </c>
-      <c r="AI326" s="43" t="s">
-        <v>1835</v>
       </c>
     </row>
     <row r="327" spans="1:35" s="12" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.3">
@@ -25785,7 +25785,7 @@
         <v>1350</v>
       </c>
       <c r="AI350" s="43" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="351" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -26537,7 +26537,7 @@
       <c r="AF364" s="15"/>
       <c r="AG364" s="16"/>
       <c r="AH364" s="43" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="AI364" s="43" t="s">
         <v>1370</v>
@@ -26596,10 +26596,10 @@
       <c r="AF365" s="15"/>
       <c r="AG365" s="16"/>
       <c r="AH365" s="43" t="s">
+        <v>1837</v>
+      </c>
+      <c r="AI365" s="43" t="s">
         <v>1838</v>
-      </c>
-      <c r="AI365" s="43" t="s">
-        <v>1839</v>
       </c>
     </row>
     <row r="366" spans="1:35" s="12" customFormat="1" ht="52.2" x14ac:dyDescent="0.3">
@@ -26707,10 +26707,10 @@
       <c r="AF367" s="15"/>
       <c r="AG367" s="16"/>
       <c r="AH367" s="43" t="s">
+        <v>1839</v>
+      </c>
+      <c r="AI367" s="43" t="s">
         <v>1840</v>
-      </c>
-      <c r="AI367" s="43" t="s">
-        <v>1841</v>
       </c>
     </row>
     <row r="368" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -26876,7 +26876,7 @@
         <v>1377</v>
       </c>
       <c r="AI370" s="43" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="371" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -26925,10 +26925,10 @@
       <c r="AF371" s="15"/>
       <c r="AG371" s="16"/>
       <c r="AH371" s="43" t="s">
+        <v>1841</v>
+      </c>
+      <c r="AI371" s="43" t="s">
         <v>1842</v>
-      </c>
-      <c r="AI371" s="43" t="s">
-        <v>1843</v>
       </c>
     </row>
     <row r="372" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -29328,10 +29328,10 @@
       <c r="AF415" s="15"/>
       <c r="AG415" s="16"/>
       <c r="AH415" s="43" t="s">
+        <v>1844</v>
+      </c>
+      <c r="AI415" s="43" t="s">
         <v>1845</v>
-      </c>
-      <c r="AI415" s="43" t="s">
-        <v>1846</v>
       </c>
     </row>
     <row r="416" spans="1:35" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -29535,7 +29535,7 @@
         <v>1449</v>
       </c>
       <c r="AI419" s="43" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="420" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -29701,7 +29701,7 @@
       <c r="AF422" s="15"/>
       <c r="AG422" s="16"/>
       <c r="AH422" s="43" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="AI422" s="43" t="s">
         <v>1454</v>
@@ -29970,10 +29970,10 @@
         <v>686</v>
       </c>
       <c r="AH427" s="43" t="s">
+        <v>1829</v>
+      </c>
+      <c r="AI427" s="43" t="s">
         <v>1830</v>
-      </c>
-      <c r="AI427" s="43" t="s">
-        <v>1831</v>
       </c>
     </row>
     <row r="428" spans="1:35" s="12" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.3">
@@ -30084,7 +30084,7 @@
         <v>1462</v>
       </c>
       <c r="AI429" s="43" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="430" spans="1:35" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -30133,7 +30133,7 @@
       <c r="AF430" s="15"/>
       <c r="AG430" s="16"/>
       <c r="AH430" s="43" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="AI430" s="43"/>
     </row>
@@ -31216,7 +31216,7 @@
         <v>692</v>
       </c>
       <c r="N451" s="14" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="O451" s="15" t="s">
         <v>5</v>

</xml_diff>